<commit_message>
discussed regarding constants and writing to excel on 29 April
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\SeleniumMar21\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEA8A78-A402-4AB7-82C1-DC8DC92EB938}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{1CB6BAC1-8DF2-492F-A988-02A80D5EC8A3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{5F09BEBF-2C3D-479A-8661-786F2BACC2EC}"/>
+    <workbookView windowHeight="13276" windowWidth="20715" xWindow="-98" xr2:uid="{5F09BEBF-2C3D-479A-8661-786F2BACC2EC}" yWindow="-98"/>
   </bookViews>
   <sheets>
-    <sheet name="BillingInfoValidation" sheetId="1" r:id="rId1"/>
+    <sheet name="BillingInfoValidation" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>RunMode</t>
   </si>
@@ -175,12 +175,19 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,20 +237,29 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -260,10 +276,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -298,7 +314,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -350,7 +366,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -461,21 +477,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -492,7 +508,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -544,31 +560,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B78BBE-F4B7-412B-8E22-F74855AC7ECA}">
-  <dimension ref="A1:L6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B78BBE-F4B7-412B-8E22-F74855AC7ECA}">
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.73046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.59765625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.3984375" collapsed="true"/>
+    <col min="10" max="11" bestFit="true" customWidth="true" width="14.73046875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.46484375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,8 +621,11 @@
       <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -643,8 +662,11 @@
       <c r="L2" t="s">
         <v>39</v>
       </c>
+      <c r="M2" t="s" s="9">
+        <v>51</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -682,7 +704,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -719,8 +741,11 @@
       <c r="L4" t="s">
         <v>41</v>
       </c>
+      <c r="M4" t="s" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -758,7 +783,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -794,18 +819,21 @@
       </c>
       <c r="L6" t="s">
         <v>43</v>
+      </c>
+      <c r="M6" t="s" s="11">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{5190FF5D-8F0C-4190-96C2-97FE3393B583}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{02CCE450-D4B4-433E-B929-60637D19F45D}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{2994B926-21B4-4C9B-B1EA-5081F9C9CB74}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{DBC196FE-E240-46C0-B645-9847758C1BB3}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{BF10EF17-2468-4341-B846-A5036D3F0425}"/>
+    <hyperlink r:id="rId1" ref="I2" xr:uid="{5190FF5D-8F0C-4190-96C2-97FE3393B583}"/>
+    <hyperlink r:id="rId2" ref="I3" xr:uid="{02CCE450-D4B4-433E-B929-60637D19F45D}"/>
+    <hyperlink r:id="rId3" ref="I4" xr:uid="{2994B926-21B4-4C9B-B1EA-5081F9C9CB74}"/>
+    <hyperlink r:id="rId4" ref="I5" xr:uid="{DBC196FE-E240-46C0-B645-9847758C1BB3}"/>
+    <hyperlink r:id="rId5" ref="I6" xr:uid="{BF10EF17-2468-4341-B846-A5036D3F0425}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
discussed about executing the code in different environments and included testing.doc which contains manual concepts.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>RunMode</t>
   </si>
@@ -240,10 +240,19 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -662,7 +671,7 @@
       <c r="L2" t="s">
         <v>39</v>
       </c>
-      <c r="M2" t="s" s="9">
+      <c r="M2" t="s" s="18">
         <v>51</v>
       </c>
     </row>
@@ -741,7 +750,7 @@
       <c r="L4" t="s">
         <v>41</v>
       </c>
-      <c r="M4" t="s" s="10">
+      <c r="M4" t="s" s="19">
         <v>51</v>
       </c>
     </row>
@@ -820,7 +829,7 @@
       <c r="L6" t="s">
         <v>43</v>
       </c>
-      <c r="M6" t="s" s="11">
+      <c r="M6" t="s" s="20">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
committing the testdata.xlsx file on 17 may 2021
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
   <si>
     <t>RunMode</t>
   </si>
@@ -240,10 +240,22 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -671,7 +683,7 @@
       <c r="L2" t="s">
         <v>39</v>
       </c>
-      <c r="M2" t="s" s="18">
+      <c r="M2" t="s" s="30">
         <v>51</v>
       </c>
     </row>
@@ -750,7 +762,7 @@
       <c r="L4" t="s">
         <v>41</v>
       </c>
-      <c r="M4" t="s" s="19">
+      <c r="M4" t="s" s="31">
         <v>51</v>
       </c>
     </row>
@@ -829,7 +841,7 @@
       <c r="L6" t="s">
         <v>43</v>
       </c>
-      <c r="M6" t="s" s="20">
+      <c r="M6" t="s" s="32">
         <v>51</v>
       </c>
     </row>

</xml_diff>